<commit_message>
Commited excel.xlsx and title.txt
</commit_message>
<xml_diff>
--- a/excel.xlsx
+++ b/excel.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ruturaj Pandit Naik\Desktop\Study\index\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{056B2A47-B759-4E4A-8384-56732125D80D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" xr2:uid="{CC15697B-5430-4E20-AC2A-E26F003E0112}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -85,7 +91,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -97,7 +103,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -144,6 +150,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -179,6 +202,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -330,13 +370,171 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31138D5F-86F4-479E-9205-C820FD0C1435}">
+  <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>